<commit_message>
refactor: contamination new function for general evaluation
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/PAH/general_eval_PAH_dw.xlsx
+++ b/inst/results/data_contam/PAH/general_eval_PAH_dw.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -558,4 +559,1320 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTUARY</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PARAMETRE_LIBELLE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>break_dates</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>last_p_value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>last_slope</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>short_last_trend</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>EAC_OSPAR_ng_gdw</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>EQS_VGE_ng_gww</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>pvalue</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>median_1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>median_2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>long_term_trend</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Fluoranthène</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>1998.250000000258</v>
+      </c>
+      <c r="D2">
+        <v>0.1105152583878463</v>
+      </c>
+      <c r="E2">
+        <v>-0.27795</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G2">
+        <v>110</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0.394</t>
+        </is>
+      </c>
+      <c r="J2">
+        <v>9.545</v>
+      </c>
+      <c r="K2">
+        <v>8.249000000000001</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Fluoranthène</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>2013.327989501731</v>
+      </c>
+      <c r="D3">
+        <v>0.4145617730512463</v>
+      </c>
+      <c r="E3">
+        <v>0.43174</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G3">
+        <v>110</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0.00665</t>
+        </is>
+      </c>
+      <c r="J3">
+        <v>16.36</v>
+      </c>
+      <c r="K3">
+        <v>7.669</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Fluoranthène</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>2011.999956919248</v>
+      </c>
+      <c r="D4">
+        <v>0.6878843369583573</v>
+      </c>
+      <c r="E4">
+        <v>0.52276</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G4">
+        <v>110</v>
+      </c>
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.0284</t>
+        </is>
+      </c>
+      <c r="J4">
+        <v>52.73</v>
+      </c>
+      <c r="K4">
+        <v>23.37</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Benzo(a)pyrène</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>2013.000202366099</v>
+      </c>
+      <c r="D5">
+        <v>0.2606021462717063</v>
+      </c>
+      <c r="E5">
+        <v>-0.23342</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G5">
+        <v>600</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0.0833</t>
+        </is>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0.2891</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Benzo(a)pyrène</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>2001.593091030837</v>
+      </c>
+      <c r="D6">
+        <v>0.02454747860055425</v>
+      </c>
+      <c r="E6">
+        <v>-0.10121</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G6">
+        <v>600</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.076</t>
+        </is>
+      </c>
+      <c r="J6">
+        <v>0.0625</v>
+      </c>
+      <c r="K6">
+        <v>0.2758</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Benzo(a)pyrène</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>2004.999629702628</v>
+      </c>
+      <c r="D7">
+        <v>0.047340441717313</v>
+      </c>
+      <c r="E7">
+        <v>-0.57358</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G7">
+        <v>600</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0.0865</t>
+        </is>
+      </c>
+      <c r="J7">
+        <v>0.5583</v>
+      </c>
+      <c r="K7">
+        <v>1.463</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Anthracène</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>2001.138442072049</v>
+      </c>
+      <c r="D8">
+        <v>0.03463788907125066</v>
+      </c>
+      <c r="E8">
+        <v>0.061766</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>↑</t>
+        </is>
+      </c>
+      <c r="G8">
+        <v>290</v>
+      </c>
+      <c r="H8">
+        <v>47.47</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0.198</t>
+        </is>
+      </c>
+      <c r="J8">
+        <v>0.3448</v>
+      </c>
+      <c r="K8">
+        <v>0.5395</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Anthracène</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>2017.999738995255</v>
+      </c>
+      <c r="D9">
+        <v>0.3204783595761644</v>
+      </c>
+      <c r="E9">
+        <v>-0.43516</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G9">
+        <v>290</v>
+      </c>
+      <c r="H9">
+        <v>47.47</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>0.946</t>
+        </is>
+      </c>
+      <c r="J9">
+        <v>0.1724</v>
+      </c>
+      <c r="K9">
+        <v>0.2393</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Anthracène</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>2010.000072141449</v>
+      </c>
+      <c r="D10">
+        <v>0.1487161894732638</v>
+      </c>
+      <c r="E10">
+        <v>0.15153</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G10">
+        <v>290</v>
+      </c>
+      <c r="H10">
+        <v>47.47</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>0.475</t>
+        </is>
+      </c>
+      <c r="J10">
+        <v>0.7413999999999999</v>
+      </c>
+      <c r="K10">
+        <v>0.8679</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Naphtalène</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>2000.000044578801</v>
+      </c>
+      <c r="D11">
+        <v>0.22472178396752</v>
+      </c>
+      <c r="E11">
+        <v>-4.3969</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G11">
+        <v>340</v>
+      </c>
+      <c r="H11">
+        <v>19.7</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.0603</t>
+        </is>
+      </c>
+      <c r="J11">
+        <v>16.03</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Naphtalène</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>2001.128277265612</v>
+      </c>
+      <c r="D12">
+        <v>0.5684221074994241</v>
+      </c>
+      <c r="E12">
+        <v>-0.31478</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G12">
+        <v>340</v>
+      </c>
+      <c r="H12">
+        <v>19.7</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>0.00902</t>
+        </is>
+      </c>
+      <c r="J12">
+        <v>4.118</v>
+      </c>
+      <c r="K12">
+        <v>0.2197</v>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Naphtalène</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>2000.000196674083</v>
+      </c>
+      <c r="D13">
+        <v>0.04388629498155386</v>
+      </c>
+      <c r="E13">
+        <v>-2.7284</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G13">
+        <v>340</v>
+      </c>
+      <c r="H13">
+        <v>19.7</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0.00388</t>
+        </is>
+      </c>
+      <c r="J13">
+        <v>5.294</v>
+      </c>
+      <c r="K13">
+        <v>0.1603</v>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Phénanthrène</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>2002.735876093304</v>
+      </c>
+      <c r="D14">
+        <v>0.7315041610253793</v>
+      </c>
+      <c r="E14">
+        <v>-0.050055</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G14">
+        <v>1700</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="J14">
+        <v>0.4353</v>
+      </c>
+      <c r="K14">
+        <v>0.3277</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Phénanthrène</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>1997.045020235592</v>
+      </c>
+      <c r="D15">
+        <v>0.5505015206618016</v>
+      </c>
+      <c r="E15">
+        <v>-0.10278</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G15">
+        <v>1700</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0.0272</t>
+        </is>
+      </c>
+      <c r="J15">
+        <v>0.9412</v>
+      </c>
+      <c r="K15">
+        <v>0.4146</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Phénanthrène</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>2003.412601153085</v>
+      </c>
+      <c r="D16">
+        <v>0.99290319879328</v>
+      </c>
+      <c r="E16">
+        <v>-0.002059</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G16">
+        <v>1700</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>0.0223</t>
+        </is>
+      </c>
+      <c r="J16">
+        <v>1.603</v>
+      </c>
+      <c r="K16">
+        <v>0.5182</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Pyrène</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>2010.000023242291</v>
+      </c>
+      <c r="D17">
+        <v>0.3258705144021785</v>
+      </c>
+      <c r="E17">
+        <v>-0.40421</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J17">
+        <v>10.05</v>
+      </c>
+      <c r="K17">
+        <v>9.640000000000001</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Pyrène</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>1998.000044748397</v>
+      </c>
+      <c r="D18">
+        <v>0.01088442336989271</v>
+      </c>
+      <c r="E18">
+        <v>-0.53873</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0.0142</t>
+        </is>
+      </c>
+      <c r="J18">
+        <v>12.25</v>
+      </c>
+      <c r="K18">
+        <v>8.648999999999999</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Pyrène</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>2000.964373849327</v>
+      </c>
+      <c r="D19">
+        <v>0.01014626593433596</v>
+      </c>
+      <c r="E19">
+        <v>-2.109</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0.0455</t>
+        </is>
+      </c>
+      <c r="J19">
+        <v>53.25</v>
+      </c>
+      <c r="K19">
+        <v>28</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Benzo(a)anthracène</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>2014.001158466421</v>
+      </c>
+      <c r="D20">
+        <v>0.5329705095224682</v>
+      </c>
+      <c r="E20">
+        <v>-0.129</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G20">
+        <v>80</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0.394</t>
+        </is>
+      </c>
+      <c r="J20">
+        <v>5.312</v>
+      </c>
+      <c r="K20">
+        <v>3.965</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Benzo(a)anthracène</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>2000.999934050714</v>
+      </c>
+      <c r="D21">
+        <v>0.001588558717288301</v>
+      </c>
+      <c r="E21">
+        <v>-0.23177</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G21">
+        <v>80</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>0.126</t>
+        </is>
+      </c>
+      <c r="J21">
+        <v>5.125</v>
+      </c>
+      <c r="K21">
+        <v>3.67</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Benzo(a)anthracène</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>1995.999796973625</v>
+      </c>
+      <c r="D22">
+        <v>0.0007603527005527267</v>
+      </c>
+      <c r="E22">
+        <v>-0.79604</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G22">
+        <v>80</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>0.475</t>
+        </is>
+      </c>
+      <c r="J22">
+        <v>23.44</v>
+      </c>
+      <c r="K22">
+        <v>16.28</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Benzo(g,h,i)pérylène</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>2013.0000041538</v>
+      </c>
+      <c r="D23">
+        <v>0.07415325534225127</v>
+      </c>
+      <c r="E23">
+        <v>0.52817</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="G23">
+        <v>110</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0.439</t>
+        </is>
+      </c>
+      <c r="J23">
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>4.828</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Benzo(g,h,i)pérylène</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>2001.999816176873</v>
+      </c>
+      <c r="D24">
+        <v>0.02916181475480942</v>
+      </c>
+      <c r="E24">
+        <v>-0.17794</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G24">
+        <v>110</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0.00451</t>
+        </is>
+      </c>
+      <c r="J24">
+        <v>5.318</v>
+      </c>
+      <c r="K24">
+        <v>3.907</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Benzo(g,h,i)pérylène</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>2001.222040692579</v>
+      </c>
+      <c r="D25">
+        <v>0.001203182481814009</v>
+      </c>
+      <c r="E25">
+        <v>-0.70266</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>↓</t>
+        </is>
+      </c>
+      <c r="G25">
+        <v>110</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0.668</t>
+        </is>
+      </c>
+      <c r="J25">
+        <v>14.09</v>
+      </c>
+      <c r="K25">
+        <v>13.1</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>→</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>blue</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>